<commit_message>
Rohan additions to records file and README.txt
</commit_message>
<xml_diff>
--- a/record_data/test.xlsx
+++ b/record_data/test.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -78,24 +78,24 @@
     <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -368,19 +368,19 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H179"/>
+  <dimension ref="A1:H180"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="14.43" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col width="24" customWidth="1" style="9" min="2" max="2"/>
-    <col width="28.86" customWidth="1" style="9" min="3" max="3"/>
-    <col width="9.710000000000001" customWidth="1" style="9" min="4" max="4"/>
-    <col width="9.140000000000001" customWidth="1" style="9" min="6" max="6"/>
-    <col width="15.86" customWidth="1" style="9" min="8" max="8"/>
+    <col customWidth="1" max="2" min="2" style="9" width="24"/>
+    <col customWidth="1" max="3" min="3" style="9" width="28.86"/>
+    <col customWidth="1" max="4" min="4" style="9" width="9.710000000000001"/>
+    <col customWidth="1" max="6" min="6" style="9" width="9.140000000000001"/>
+    <col customWidth="1" max="8" min="8" style="9" width="15.86"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6272,40 +6272,74 @@
       </c>
     </row>
     <row r="179">
-      <c r="A179" t="inlineStr"/>
-      <c r="B179" t="inlineStr">
+      <c r="A179" s="0" t="inlineStr"/>
+      <c r="B179" s="0" t="inlineStr">
         <is>
           <t>E'voke</t>
         </is>
       </c>
-      <c r="C179" t="inlineStr">
+      <c r="C179" s="0" t="inlineStr">
         <is>
           <t>Runaway</t>
         </is>
       </c>
-      <c r="D179" t="inlineStr">
-        <is>
-          <t>EP</t>
-        </is>
-      </c>
-      <c r="E179" t="inlineStr">
+      <c r="D179" s="0" t="inlineStr">
+        <is>
+          <t>EP</t>
+        </is>
+      </c>
+      <c r="E179" s="0" t="inlineStr">
         <is>
           <t>Progressive House, House</t>
         </is>
       </c>
-      <c r="F179" t="n">
+      <c r="F179" s="0" t="n">
         <v>1995</v>
       </c>
-      <c r="G179" t="inlineStr">
+      <c r="G179" s="0" t="inlineStr">
         <is>
           <t>G</t>
         </is>
       </c>
-      <c r="H179" t="n">
+      <c r="H179" s="0" t="n">
         <v>3.99</v>
       </c>
     </row>
+    <row r="180">
+      <c r="A180" t="inlineStr"/>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>I*Levels*</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>I*Levels</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>EP</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>Deep House, Tech House</t>
+        </is>
+      </c>
+      <c r="F180" t="n">
+        <v>1995</v>
+      </c>
+      <c r="G180" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="H180" t="n">
+        <v>4.49</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>